<commit_message>
Monday Aug 25 22:05
</commit_message>
<xml_diff>
--- a/MultiDayConcat/concat_days.xlsx
+++ b/MultiDayConcat/concat_days.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miguel_barron/Documents/Research/ALAB/Code/alab_code/MultiDayConcat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D386DCF-0AFF-7F45-A788-EC2A780D1E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F2E172-0667-E141-B9FC-58CCAB09DEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="760" windowWidth="27400" windowHeight="11300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Day</t>
   </si>
@@ -28,40 +28,7 @@
     <t>Path</t>
   </si>
   <si>
-    <t>Day 4</t>
-  </si>
-  <si>
-    <t>Day 5</t>
-  </si>
-  <si>
-    <t>Day 6</t>
-  </si>
-  <si>
-    <t>Day 7</t>
-  </si>
-  <si>
-    <t>Day 8</t>
-  </si>
-  <si>
-    <t>Day 9</t>
-  </si>
-  <si>
-    <t>/Volumes/ASA_Lab/Data/Julia/ATNRSC/CCH_9day/ZA03/concatData/concatEphys/Day 4</t>
-  </si>
-  <si>
-    <t>/Volumes/ASA_Lab/Data/Julia/ATNRSC/CCH_9day/ZA03/concatData/concatEphys/Day 5</t>
-  </si>
-  <si>
-    <t>/Volumes/ASA_Lab/Data/Julia/ATNRSC/CCH_9day/ZA03/concatData/concatEphys/Day 6</t>
-  </si>
-  <si>
-    <t>/Volumes/ASA_Lab/Data/Julia/ATNRSC/CCH_9day/ZA03/concatData/concatEphys/Day 7</t>
-  </si>
-  <si>
-    <t>/Volumes/ASA_Lab/Data/Julia/ATNRSC/CCH_9day/ZA03/concatData/concatEphys/Day 8</t>
-  </si>
-  <si>
-    <t>/Volumes/ASA_Lab/Data/Julia/ATNRSC/CCH_9day/ZA03/concatData/concatEphys/Day 9</t>
+    <t>/Users/miguel_barron/Downloads/concatEphys/03312025</t>
   </si>
 </sst>
 </file>
@@ -412,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="244" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -432,51 +399,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
+      <c r="A2">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>